<commit_message>
minor fix tcl, excel
</commit_message>
<xml_diff>
--- a/docs/ram.xlsx
+++ b/docs/ram.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\SS\fpga\fft\fht\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\fpga\fht\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="11790"/>
+    <workbookView minimized="1" xWindow="0" yWindow="0" windowWidth="19200" windowHeight="11790"/>
   </bookViews>
   <sheets>
     <sheet name="Лист1" sheetId="1" r:id="rId1"/>
@@ -24,12 +24,15 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
   <si>
     <t>FHT:</t>
   </si>
   <si>
     <t>FFT:</t>
+  </si>
+  <si>
+    <t>addr</t>
   </si>
 </sst>
 </file>
@@ -69,7 +72,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -77,15 +80,57 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
@@ -369,7 +414,7 @@
   <dimension ref="A1:X34"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K9" sqref="K9"/>
+      <selection activeCell="B22" sqref="B22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -787,7 +832,7 @@
         <v>1.49611189188504</v>
       </c>
     </row>
-    <row r="17" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="2">
         <v>-1.0516649878667399</v>
       </c>
@@ -814,6 +859,11 @@
         <v>9.6777338124935905</v>
       </c>
     </row>
+    <row r="18" spans="1:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E18" s="6" t="s">
+        <v>2</v>
+      </c>
+    </row>
     <row r="19" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A19" s="2">
         <v>0</v>
@@ -827,7 +877,9 @@
       <c r="D19" s="2">
         <v>48</v>
       </c>
-      <c r="E19" s="2"/>
+      <c r="E19" s="4">
+        <v>0</v>
+      </c>
       <c r="F19" s="2">
         <v>0</v>
       </c>
@@ -903,7 +955,9 @@
       <c r="D20" s="2">
         <v>56</v>
       </c>
-      <c r="E20" s="2"/>
+      <c r="E20" s="4">
+        <v>1</v>
+      </c>
       <c r="F20" s="2">
         <v>4</v>
       </c>
@@ -979,7 +1033,9 @@
       <c r="D21" s="2">
         <v>52</v>
       </c>
-      <c r="E21" s="2"/>
+      <c r="E21" s="4">
+        <v>2</v>
+      </c>
       <c r="F21" s="2">
         <v>8</v>
       </c>
@@ -1055,7 +1111,9 @@
       <c r="D22" s="2">
         <v>60</v>
       </c>
-      <c r="E22" s="2"/>
+      <c r="E22" s="4">
+        <v>3</v>
+      </c>
       <c r="F22" s="2">
         <v>12</v>
       </c>
@@ -1131,7 +1189,9 @@
       <c r="D23" s="2">
         <v>50</v>
       </c>
-      <c r="E23" s="2"/>
+      <c r="E23" s="4">
+        <v>4</v>
+      </c>
       <c r="F23" s="2">
         <v>16</v>
       </c>
@@ -1207,7 +1267,9 @@
       <c r="D24" s="2">
         <v>58</v>
       </c>
-      <c r="E24" s="2"/>
+      <c r="E24" s="4">
+        <v>5</v>
+      </c>
       <c r="F24" s="2">
         <v>20</v>
       </c>
@@ -1283,7 +1345,9 @@
       <c r="D25" s="2">
         <v>54</v>
       </c>
-      <c r="E25" s="2"/>
+      <c r="E25" s="4">
+        <v>6</v>
+      </c>
       <c r="F25" s="2">
         <v>24</v>
       </c>
@@ -1359,7 +1423,9 @@
       <c r="D26" s="2">
         <v>62</v>
       </c>
-      <c r="E26" s="2"/>
+      <c r="E26" s="4">
+        <v>7</v>
+      </c>
       <c r="F26" s="2">
         <v>28</v>
       </c>
@@ -1435,7 +1501,9 @@
       <c r="D27" s="2">
         <v>49</v>
       </c>
-      <c r="E27" s="2"/>
+      <c r="E27" s="4">
+        <v>8</v>
+      </c>
       <c r="F27" s="2">
         <v>32</v>
       </c>
@@ -1511,7 +1579,9 @@
       <c r="D28" s="2">
         <v>57</v>
       </c>
-      <c r="E28" s="2"/>
+      <c r="E28" s="4">
+        <v>9</v>
+      </c>
       <c r="F28" s="2">
         <v>36</v>
       </c>
@@ -1587,7 +1657,9 @@
       <c r="D29" s="2">
         <v>53</v>
       </c>
-      <c r="E29" s="2"/>
+      <c r="E29" s="4">
+        <v>10</v>
+      </c>
       <c r="F29" s="2">
         <v>40</v>
       </c>
@@ -1663,7 +1735,9 @@
       <c r="D30" s="2">
         <v>61</v>
       </c>
-      <c r="E30" s="2"/>
+      <c r="E30" s="4">
+        <v>11</v>
+      </c>
       <c r="F30" s="2">
         <v>44</v>
       </c>
@@ -1739,6 +1813,9 @@
       <c r="D31" s="2">
         <v>51</v>
       </c>
+      <c r="E31" s="4">
+        <v>12</v>
+      </c>
       <c r="F31" s="2">
         <v>48</v>
       </c>
@@ -1813,6 +1890,9 @@
       <c r="D32" s="2">
         <v>59</v>
       </c>
+      <c r="E32" s="4">
+        <v>13</v>
+      </c>
       <c r="F32" s="2">
         <v>52</v>
       </c>
@@ -1887,6 +1967,9 @@
       <c r="D33" s="2">
         <v>55</v>
       </c>
+      <c r="E33" s="4">
+        <v>14</v>
+      </c>
       <c r="F33" s="2">
         <v>56</v>
       </c>
@@ -1948,7 +2031,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="34" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A34" s="2">
         <v>15</v>
       </c>
@@ -1960,6 +2043,9 @@
       </c>
       <c r="D34" s="2">
         <v>63</v>
+      </c>
+      <c r="E34" s="5">
+        <v>15</v>
       </c>
       <c r="F34" s="2">
         <v>60</v>

</xml_diff>

<commit_message>
fix verilog, tcl, tb, excel
</commit_message>
<xml_diff>
--- a/docs/ram.xlsx
+++ b/docs/ram.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView minimized="1" xWindow="0" yWindow="0" windowWidth="19200" windowHeight="11790"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="11790"/>
   </bookViews>
   <sheets>
     <sheet name="Лист1" sheetId="1" r:id="rId1"/>
@@ -72,7 +72,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="4">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -119,11 +119,24 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -131,6 +144,10 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
@@ -414,7 +431,7 @@
   <dimension ref="A1:X34"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B22" sqref="B22"/>
+      <selection activeCell="T15" sqref="T15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -892,7 +909,10 @@
       <c r="I19" s="2">
         <v>3</v>
       </c>
-      <c r="J19" s="2"/>
+      <c r="J19" s="7" t="str">
+        <f>DEC2BIN(E19,4)</f>
+        <v>0000</v>
+      </c>
       <c r="K19" t="str">
         <f>DEC2BIN(A19,6)</f>
         <v>000000</v>
@@ -909,6 +929,10 @@
         <f t="shared" si="0"/>
         <v>110000</v>
       </c>
+      <c r="O19" s="10">
+        <f>SUMPRODUCT(MID($J19,{1;2;3;4},1)*10^{0;1;2;3})</f>
+        <v>0</v>
+      </c>
       <c r="P19">
         <f>SUMPRODUCT(MID($K19,{1;2;3;4;5;6},1)*10^{0;1;2;3;4;5})</f>
         <v>0</v>
@@ -925,6 +949,10 @@
         <f>SUMPRODUCT(MID($N19,{1;2;3;4;5;6},1)*10^{0;1;2;3;4;5})</f>
         <v>11</v>
       </c>
+      <c r="T19" s="10">
+        <f>BIN2DEC(O19)</f>
+        <v>0</v>
+      </c>
       <c r="U19">
         <f>BIN2DEC(P19)</f>
         <v>0</v>
@@ -970,9 +998,12 @@
       <c r="I20" s="2">
         <v>7</v>
       </c>
-      <c r="J20" s="2"/>
+      <c r="J20" s="4" t="str">
+        <f t="shared" ref="J20:J34" si="2">DEC2BIN(E20,4)</f>
+        <v>0001</v>
+      </c>
       <c r="K20" t="str">
-        <f t="shared" ref="K20:K34" si="2">DEC2BIN(A20,6)</f>
+        <f t="shared" ref="K20:K34" si="3">DEC2BIN(A20,6)</f>
         <v>001000</v>
       </c>
       <c r="L20" t="str">
@@ -986,6 +1017,10 @@
       <c r="N20" t="str">
         <f t="shared" si="0"/>
         <v>111000</v>
+      </c>
+      <c r="O20" s="8">
+        <f>SUMPRODUCT(MID($J20,{1;2;3;4},1)*10^{0;1;2;3})</f>
+        <v>1000</v>
       </c>
       <c r="P20">
         <f>SUMPRODUCT(MID($K20,{1;2;3;4;5;6},1)*10^{0;1;2;3;4;5})</f>
@@ -1003,8 +1038,12 @@
         <f>SUMPRODUCT(MID($N20,{1;2;3;4;5;6},1)*10^{0;1;2;3;4;5})</f>
         <v>111</v>
       </c>
+      <c r="T20" s="8">
+        <f t="shared" ref="T20:T34" si="4">BIN2DEC(O20)</f>
+        <v>8</v>
+      </c>
       <c r="U20">
-        <f t="shared" ref="U20:U34" si="3">BIN2DEC(P20)</f>
+        <f t="shared" ref="U20:U34" si="5">BIN2DEC(P20)</f>
         <v>4</v>
       </c>
       <c r="V20">
@@ -1048,9 +1087,12 @@
       <c r="I21" s="2">
         <v>11</v>
       </c>
-      <c r="J21" s="2"/>
+      <c r="J21" s="4" t="str">
+        <f t="shared" si="2"/>
+        <v>0010</v>
+      </c>
       <c r="K21" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>000100</v>
       </c>
       <c r="L21" t="str">
@@ -1064,6 +1106,10 @@
       <c r="N21" t="str">
         <f t="shared" si="0"/>
         <v>110100</v>
+      </c>
+      <c r="O21" s="8">
+        <f>SUMPRODUCT(MID($J21,{1;2;3;4},1)*10^{0;1;2;3})</f>
+        <v>100</v>
       </c>
       <c r="P21">
         <f>SUMPRODUCT(MID($K21,{1;2;3;4;5;6},1)*10^{0;1;2;3;4;5})</f>
@@ -1081,8 +1127,12 @@
         <f>SUMPRODUCT(MID($N21,{1;2;3;4;5;6},1)*10^{0;1;2;3;4;5})</f>
         <v>1011</v>
       </c>
+      <c r="T21" s="8">
+        <f t="shared" si="4"/>
+        <v>4</v>
+      </c>
       <c r="U21">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>8</v>
       </c>
       <c r="V21">
@@ -1126,9 +1176,12 @@
       <c r="I22" s="2">
         <v>15</v>
       </c>
-      <c r="J22" s="2"/>
+      <c r="J22" s="4" t="str">
+        <f t="shared" si="2"/>
+        <v>0011</v>
+      </c>
       <c r="K22" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>001100</v>
       </c>
       <c r="L22" t="str">
@@ -1142,6 +1195,10 @@
       <c r="N22" t="str">
         <f t="shared" si="0"/>
         <v>111100</v>
+      </c>
+      <c r="O22" s="8">
+        <f>SUMPRODUCT(MID($J22,{1;2;3;4},1)*10^{0;1;2;3})</f>
+        <v>1100</v>
       </c>
       <c r="P22">
         <f>SUMPRODUCT(MID($K22,{1;2;3;4;5;6},1)*10^{0;1;2;3;4;5})</f>
@@ -1159,8 +1216,12 @@
         <f>SUMPRODUCT(MID($N22,{1;2;3;4;5;6},1)*10^{0;1;2;3;4;5})</f>
         <v>1111</v>
       </c>
+      <c r="T22" s="8">
+        <f t="shared" si="4"/>
+        <v>12</v>
+      </c>
       <c r="U22">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>12</v>
       </c>
       <c r="V22">
@@ -1204,9 +1265,12 @@
       <c r="I23" s="2">
         <v>19</v>
       </c>
-      <c r="J23" s="2"/>
+      <c r="J23" s="4" t="str">
+        <f t="shared" si="2"/>
+        <v>0100</v>
+      </c>
       <c r="K23" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>000010</v>
       </c>
       <c r="L23" t="str">
@@ -1220,6 +1284,10 @@
       <c r="N23" t="str">
         <f t="shared" si="0"/>
         <v>110010</v>
+      </c>
+      <c r="O23" s="8">
+        <f>SUMPRODUCT(MID($J23,{1;2;3;4},1)*10^{0;1;2;3})</f>
+        <v>10</v>
       </c>
       <c r="P23">
         <f>SUMPRODUCT(MID($K23,{1;2;3;4;5;6},1)*10^{0;1;2;3;4;5})</f>
@@ -1237,8 +1305,12 @@
         <f>SUMPRODUCT(MID($N23,{1;2;3;4;5;6},1)*10^{0;1;2;3;4;5})</f>
         <v>10011</v>
       </c>
+      <c r="T23" s="8">
+        <f t="shared" si="4"/>
+        <v>2</v>
+      </c>
       <c r="U23">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>16</v>
       </c>
       <c r="V23">
@@ -1282,9 +1354,12 @@
       <c r="I24" s="2">
         <v>23</v>
       </c>
-      <c r="J24" s="2"/>
+      <c r="J24" s="4" t="str">
+        <f t="shared" si="2"/>
+        <v>0101</v>
+      </c>
       <c r="K24" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>001010</v>
       </c>
       <c r="L24" t="str">
@@ -1298,6 +1373,10 @@
       <c r="N24" t="str">
         <f t="shared" si="0"/>
         <v>111010</v>
+      </c>
+      <c r="O24" s="8">
+        <f>SUMPRODUCT(MID($J24,{1;2;3;4},1)*10^{0;1;2;3})</f>
+        <v>1010</v>
       </c>
       <c r="P24">
         <f>SUMPRODUCT(MID($K24,{1;2;3;4;5;6},1)*10^{0;1;2;3;4;5})</f>
@@ -1315,8 +1394,12 @@
         <f>SUMPRODUCT(MID($N24,{1;2;3;4;5;6},1)*10^{0;1;2;3;4;5})</f>
         <v>10111</v>
       </c>
+      <c r="T24" s="8">
+        <f t="shared" si="4"/>
+        <v>10</v>
+      </c>
       <c r="U24">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>20</v>
       </c>
       <c r="V24">
@@ -1360,9 +1443,12 @@
       <c r="I25" s="2">
         <v>27</v>
       </c>
-      <c r="J25" s="2"/>
+      <c r="J25" s="4" t="str">
+        <f t="shared" si="2"/>
+        <v>0110</v>
+      </c>
       <c r="K25" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>000110</v>
       </c>
       <c r="L25" t="str">
@@ -1376,6 +1462,10 @@
       <c r="N25" t="str">
         <f t="shared" si="0"/>
         <v>110110</v>
+      </c>
+      <c r="O25" s="8">
+        <f>SUMPRODUCT(MID($J25,{1;2;3;4},1)*10^{0;1;2;3})</f>
+        <v>110</v>
       </c>
       <c r="P25">
         <f>SUMPRODUCT(MID($K25,{1;2;3;4;5;6},1)*10^{0;1;2;3;4;5})</f>
@@ -1393,8 +1483,12 @@
         <f>SUMPRODUCT(MID($N25,{1;2;3;4;5;6},1)*10^{0;1;2;3;4;5})</f>
         <v>11011</v>
       </c>
+      <c r="T25" s="8">
+        <f t="shared" si="4"/>
+        <v>6</v>
+      </c>
       <c r="U25">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>24</v>
       </c>
       <c r="V25">
@@ -1438,9 +1532,12 @@
       <c r="I26" s="2">
         <v>31</v>
       </c>
-      <c r="J26" s="2"/>
+      <c r="J26" s="4" t="str">
+        <f t="shared" si="2"/>
+        <v>0111</v>
+      </c>
       <c r="K26" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>001110</v>
       </c>
       <c r="L26" t="str">
@@ -1454,6 +1551,10 @@
       <c r="N26" t="str">
         <f t="shared" si="0"/>
         <v>111110</v>
+      </c>
+      <c r="O26" s="8">
+        <f>SUMPRODUCT(MID($J26,{1;2;3;4},1)*10^{0;1;2;3})</f>
+        <v>1110</v>
       </c>
       <c r="P26">
         <f>SUMPRODUCT(MID($K26,{1;2;3;4;5;6},1)*10^{0;1;2;3;4;5})</f>
@@ -1471,8 +1572,12 @@
         <f>SUMPRODUCT(MID($N26,{1;2;3;4;5;6},1)*10^{0;1;2;3;4;5})</f>
         <v>11111</v>
       </c>
+      <c r="T26" s="8">
+        <f t="shared" si="4"/>
+        <v>14</v>
+      </c>
       <c r="U26">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>28</v>
       </c>
       <c r="V26">
@@ -1516,9 +1621,12 @@
       <c r="I27" s="2">
         <v>35</v>
       </c>
-      <c r="J27" s="2"/>
+      <c r="J27" s="4" t="str">
+        <f t="shared" si="2"/>
+        <v>1000</v>
+      </c>
       <c r="K27" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>000001</v>
       </c>
       <c r="L27" t="str">
@@ -1532,6 +1640,10 @@
       <c r="N27" t="str">
         <f t="shared" si="0"/>
         <v>110001</v>
+      </c>
+      <c r="O27" s="8">
+        <f>SUMPRODUCT(MID($J27,{1;2;3;4},1)*10^{0;1;2;3})</f>
+        <v>1</v>
       </c>
       <c r="P27">
         <f>SUMPRODUCT(MID($K27,{1;2;3;4;5;6},1)*10^{0;1;2;3;4;5})</f>
@@ -1549,8 +1661,12 @@
         <f>SUMPRODUCT(MID($N27,{1;2;3;4;5;6},1)*10^{0;1;2;3;4;5})</f>
         <v>100011</v>
       </c>
+      <c r="T27" s="8">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
       <c r="U27">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>32</v>
       </c>
       <c r="V27">
@@ -1594,9 +1710,12 @@
       <c r="I28" s="2">
         <v>39</v>
       </c>
-      <c r="J28" s="2"/>
+      <c r="J28" s="4" t="str">
+        <f t="shared" si="2"/>
+        <v>1001</v>
+      </c>
       <c r="K28" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>001001</v>
       </c>
       <c r="L28" t="str">
@@ -1610,6 +1729,10 @@
       <c r="N28" t="str">
         <f t="shared" si="0"/>
         <v>111001</v>
+      </c>
+      <c r="O28" s="8">
+        <f>SUMPRODUCT(MID($J28,{1;2;3;4},1)*10^{0;1;2;3})</f>
+        <v>1001</v>
       </c>
       <c r="P28">
         <f>SUMPRODUCT(MID($K28,{1;2;3;4;5;6},1)*10^{0;1;2;3;4;5})</f>
@@ -1627,8 +1750,12 @@
         <f>SUMPRODUCT(MID($N28,{1;2;3;4;5;6},1)*10^{0;1;2;3;4;5})</f>
         <v>100111</v>
       </c>
+      <c r="T28" s="8">
+        <f t="shared" si="4"/>
+        <v>9</v>
+      </c>
       <c r="U28">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>36</v>
       </c>
       <c r="V28">
@@ -1672,9 +1799,12 @@
       <c r="I29" s="2">
         <v>43</v>
       </c>
-      <c r="J29" s="2"/>
+      <c r="J29" s="4" t="str">
+        <f t="shared" si="2"/>
+        <v>1010</v>
+      </c>
       <c r="K29" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>000101</v>
       </c>
       <c r="L29" t="str">
@@ -1688,6 +1818,10 @@
       <c r="N29" t="str">
         <f t="shared" si="0"/>
         <v>110101</v>
+      </c>
+      <c r="O29" s="8">
+        <f>SUMPRODUCT(MID($J29,{1;2;3;4},1)*10^{0;1;2;3})</f>
+        <v>101</v>
       </c>
       <c r="P29">
         <f>SUMPRODUCT(MID($K29,{1;2;3;4;5;6},1)*10^{0;1;2;3;4;5})</f>
@@ -1705,8 +1839,12 @@
         <f>SUMPRODUCT(MID($N29,{1;2;3;4;5;6},1)*10^{0;1;2;3;4;5})</f>
         <v>101011</v>
       </c>
+      <c r="T29" s="8">
+        <f t="shared" si="4"/>
+        <v>5</v>
+      </c>
       <c r="U29">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>40</v>
       </c>
       <c r="V29">
@@ -1750,9 +1888,12 @@
       <c r="I30" s="2">
         <v>47</v>
       </c>
-      <c r="J30" s="2"/>
+      <c r="J30" s="4" t="str">
+        <f t="shared" si="2"/>
+        <v>1011</v>
+      </c>
       <c r="K30" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>001101</v>
       </c>
       <c r="L30" t="str">
@@ -1766,6 +1907,10 @@
       <c r="N30" t="str">
         <f t="shared" si="0"/>
         <v>111101</v>
+      </c>
+      <c r="O30" s="8">
+        <f>SUMPRODUCT(MID($J30,{1;2;3;4},1)*10^{0;1;2;3})</f>
+        <v>1101</v>
       </c>
       <c r="P30">
         <f>SUMPRODUCT(MID($K30,{1;2;3;4;5;6},1)*10^{0;1;2;3;4;5})</f>
@@ -1783,8 +1928,12 @@
         <f>SUMPRODUCT(MID($N30,{1;2;3;4;5;6},1)*10^{0;1;2;3;4;5})</f>
         <v>101111</v>
       </c>
+      <c r="T30" s="8">
+        <f t="shared" si="4"/>
+        <v>13</v>
+      </c>
       <c r="U30">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>44</v>
       </c>
       <c r="V30">
@@ -1828,8 +1977,12 @@
       <c r="I31" s="2">
         <v>51</v>
       </c>
+      <c r="J31" s="4" t="str">
+        <f t="shared" si="2"/>
+        <v>1100</v>
+      </c>
       <c r="K31" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>000011</v>
       </c>
       <c r="L31" t="str">
@@ -1843,6 +1996,10 @@
       <c r="N31" t="str">
         <f t="shared" si="0"/>
         <v>110011</v>
+      </c>
+      <c r="O31" s="8">
+        <f>SUMPRODUCT(MID($J31,{1;2;3;4},1)*10^{0;1;2;3})</f>
+        <v>11</v>
       </c>
       <c r="P31">
         <f>SUMPRODUCT(MID($K31,{1;2;3;4;5;6},1)*10^{0;1;2;3;4;5})</f>
@@ -1860,8 +2017,12 @@
         <f>SUMPRODUCT(MID($N31,{1;2;3;4;5;6},1)*10^{0;1;2;3;4;5})</f>
         <v>110011</v>
       </c>
+      <c r="T31" s="8">
+        <f t="shared" si="4"/>
+        <v>3</v>
+      </c>
       <c r="U31">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>48</v>
       </c>
       <c r="V31">
@@ -1905,8 +2066,12 @@
       <c r="I32" s="2">
         <v>55</v>
       </c>
+      <c r="J32" s="4" t="str">
+        <f t="shared" si="2"/>
+        <v>1101</v>
+      </c>
       <c r="K32" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>001011</v>
       </c>
       <c r="L32" t="str">
@@ -1920,6 +2085,10 @@
       <c r="N32" t="str">
         <f t="shared" si="0"/>
         <v>111011</v>
+      </c>
+      <c r="O32" s="8">
+        <f>SUMPRODUCT(MID($J32,{1;2;3;4},1)*10^{0;1;2;3})</f>
+        <v>1011</v>
       </c>
       <c r="P32">
         <f>SUMPRODUCT(MID($K32,{1;2;3;4;5;6},1)*10^{0;1;2;3;4;5})</f>
@@ -1937,8 +2106,12 @@
         <f>SUMPRODUCT(MID($N32,{1;2;3;4;5;6},1)*10^{0;1;2;3;4;5})</f>
         <v>110111</v>
       </c>
+      <c r="T32" s="8">
+        <f t="shared" si="4"/>
+        <v>11</v>
+      </c>
       <c r="U32">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>52</v>
       </c>
       <c r="V32">
@@ -1982,8 +2155,12 @@
       <c r="I33" s="2">
         <v>59</v>
       </c>
+      <c r="J33" s="4" t="str">
+        <f t="shared" si="2"/>
+        <v>1110</v>
+      </c>
       <c r="K33" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>000111</v>
       </c>
       <c r="L33" t="str">
@@ -1997,6 +2174,10 @@
       <c r="N33" t="str">
         <f t="shared" si="0"/>
         <v>110111</v>
+      </c>
+      <c r="O33" s="8">
+        <f>SUMPRODUCT(MID($J33,{1;2;3;4},1)*10^{0;1;2;3})</f>
+        <v>111</v>
       </c>
       <c r="P33">
         <f>SUMPRODUCT(MID($K33,{1;2;3;4;5;6},1)*10^{0;1;2;3;4;5})</f>
@@ -2014,8 +2195,12 @@
         <f>SUMPRODUCT(MID($N33,{1;2;3;4;5;6},1)*10^{0;1;2;3;4;5})</f>
         <v>111011</v>
       </c>
+      <c r="T33" s="8">
+        <f t="shared" si="4"/>
+        <v>7</v>
+      </c>
       <c r="U33">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>56</v>
       </c>
       <c r="V33">
@@ -2059,8 +2244,12 @@
       <c r="I34" s="2">
         <v>63</v>
       </c>
+      <c r="J34" s="5" t="str">
+        <f t="shared" si="2"/>
+        <v>1111</v>
+      </c>
       <c r="K34" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>001111</v>
       </c>
       <c r="L34" t="str">
@@ -2074,6 +2263,10 @@
       <c r="N34" t="str">
         <f t="shared" si="0"/>
         <v>111111</v>
+      </c>
+      <c r="O34" s="9">
+        <f>SUMPRODUCT(MID($J34,{1;2;3;4},1)*10^{0;1;2;3})</f>
+        <v>1111</v>
       </c>
       <c r="P34">
         <f>SUMPRODUCT(MID($K34,{1;2;3;4;5;6},1)*10^{0;1;2;3;4;5})</f>
@@ -2091,8 +2284,12 @@
         <f>SUMPRODUCT(MID($N34,{1;2;3;4;5;6},1)*10^{0;1;2;3;4;5})</f>
         <v>111111</v>
       </c>
+      <c r="T34" s="9">
+        <f t="shared" si="4"/>
+        <v>15</v>
+      </c>
       <c r="U34">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>60</v>
       </c>
       <c r="V34">

</xml_diff>

<commit_message>
minor, display IFHT data in fht_tb
</commit_message>
<xml_diff>
--- a/docs/ram.xlsx
+++ b/docs/ram.xlsx
@@ -428,10 +428,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:X34"/>
+  <dimension ref="A1:X38"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="T15" sqref="T15"/>
+      <selection activeCell="Q3" sqref="Q3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2305,6 +2305,7 @@
         <v>63</v>
       </c>
     </row>
+    <row r="38" spans="1:24" ht="17.25" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>

</xml_diff>

<commit_message>
add separate generate IMP POS and NEG RAM for check conv
</commit_message>
<xml_diff>
--- a/docs/ram.xlsx
+++ b/docs/ram.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\fpga\fht\docs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\work\fpga\fht\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="58">
   <si>
     <t>FHT:</t>
   </si>
@@ -32,7 +32,172 @@
     <t>FFT:</t>
   </si>
   <si>
-    <t>addr</t>
+    <t>0 0</t>
+  </si>
+  <si>
+    <t>1 1</t>
+  </si>
+  <si>
+    <t>0 3</t>
+  </si>
+  <si>
+    <t>0 1</t>
+  </si>
+  <si>
+    <t>0 2</t>
+  </si>
+  <si>
+    <t>1 3</t>
+  </si>
+  <si>
+    <t>1 2</t>
+  </si>
+  <si>
+    <t>1 0</t>
+  </si>
+  <si>
+    <t>3 3</t>
+  </si>
+  <si>
+    <t>3 2</t>
+  </si>
+  <si>
+    <t>3 1</t>
+  </si>
+  <si>
+    <t>3 0</t>
+  </si>
+  <si>
+    <t>2 3</t>
+  </si>
+  <si>
+    <t>2 2</t>
+  </si>
+  <si>
+    <t>2 1</t>
+  </si>
+  <si>
+    <t>2 0</t>
+  </si>
+  <si>
+    <t>7 3</t>
+  </si>
+  <si>
+    <t>7 2</t>
+  </si>
+  <si>
+    <t>7 1</t>
+  </si>
+  <si>
+    <t>7 0</t>
+  </si>
+  <si>
+    <t>6 3</t>
+  </si>
+  <si>
+    <t>6 2</t>
+  </si>
+  <si>
+    <t>6 1</t>
+  </si>
+  <si>
+    <t>6 0</t>
+  </si>
+  <si>
+    <t>5 3</t>
+  </si>
+  <si>
+    <t>5 2</t>
+  </si>
+  <si>
+    <t>5 1</t>
+  </si>
+  <si>
+    <t>5 0</t>
+  </si>
+  <si>
+    <t>4 3</t>
+  </si>
+  <si>
+    <t>4 2</t>
+  </si>
+  <si>
+    <t>4 1</t>
+  </si>
+  <si>
+    <t>4 0</t>
+  </si>
+  <si>
+    <t>15 3</t>
+  </si>
+  <si>
+    <t>15 2</t>
+  </si>
+  <si>
+    <t>15 1</t>
+  </si>
+  <si>
+    <t>15 0</t>
+  </si>
+  <si>
+    <t>14 3</t>
+  </si>
+  <si>
+    <t>14 2</t>
+  </si>
+  <si>
+    <t>14 1</t>
+  </si>
+  <si>
+    <t>14 0</t>
+  </si>
+  <si>
+    <t>13 2</t>
+  </si>
+  <si>
+    <t>13 3</t>
+  </si>
+  <si>
+    <t>13 1</t>
+  </si>
+  <si>
+    <t>13 0</t>
+  </si>
+  <si>
+    <t>12 3</t>
+  </si>
+  <si>
+    <t>12 2</t>
+  </si>
+  <si>
+    <t>12 1</t>
+  </si>
+  <si>
+    <t>12 0</t>
+  </si>
+  <si>
+    <t>11 3</t>
+  </si>
+  <si>
+    <t>10 3</t>
+  </si>
+  <si>
+    <t>9 3</t>
+  </si>
+  <si>
+    <t>8 3</t>
+  </si>
+  <si>
+    <t>bank/addr</t>
+  </si>
+  <si>
+    <t>inv num</t>
+  </si>
+  <si>
+    <t>row-col</t>
+  </si>
+  <si>
+    <t>for imp pos/neg</t>
   </si>
 </sst>
 </file>
@@ -72,7 +237,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="5">
+  <borders count="16">
     <border>
       <left/>
       <right/>
@@ -132,11 +297,128 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -148,6 +430,20 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
@@ -431,20 +727,44 @@
   <dimension ref="A1:X38"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="Q3" sqref="Q3"/>
+      <selection activeCell="Q2" sqref="Q2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="5" max="5" width="9.85546875" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="F1" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="K1" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="L1" s="23">
+        <v>0</v>
+      </c>
+      <c r="M1" s="24">
+        <v>1</v>
+      </c>
+      <c r="N1" s="24">
+        <v>2</v>
+      </c>
+      <c r="O1" s="12">
+        <v>3</v>
+      </c>
+      <c r="P1" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="2" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A2" s="2">
         <v>31.5</v>
       </c>
@@ -470,8 +790,38 @@
       <c r="I2" s="2">
         <v>-3.8707262027074898</v>
       </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="K2" s="7">
+        <v>0</v>
+      </c>
+      <c r="L2" s="15">
+        <v>0</v>
+      </c>
+      <c r="M2" s="16">
+        <f t="shared" ref="M2:O17" si="0">64-B19</f>
+        <v>32</v>
+      </c>
+      <c r="N2" s="16">
+        <f t="shared" si="0"/>
+        <v>48</v>
+      </c>
+      <c r="O2" s="17">
+        <f t="shared" si="0"/>
+        <v>16</v>
+      </c>
+      <c r="Q2" s="15" t="s">
+        <v>2</v>
+      </c>
+      <c r="R2" s="16" t="s">
+        <v>5</v>
+      </c>
+      <c r="S2" s="16" t="s">
+        <v>4</v>
+      </c>
+      <c r="T2" s="17" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="3" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A3" s="2">
         <v>-1.7071067811865499</v>
       </c>
@@ -497,8 +847,39 @@
       <c r="I3" s="2">
         <v>-1.8974063862452399</v>
       </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="K3" s="4">
+        <v>1</v>
+      </c>
+      <c r="L3" s="18">
+        <f t="shared" ref="L3:L17" si="1">64-A20</f>
+        <v>56</v>
+      </c>
+      <c r="M3" s="11">
+        <f t="shared" si="0"/>
+        <v>24</v>
+      </c>
+      <c r="N3" s="11">
+        <f t="shared" si="0"/>
+        <v>40</v>
+      </c>
+      <c r="O3" s="19">
+        <f t="shared" si="0"/>
+        <v>8</v>
+      </c>
+      <c r="Q3" s="18" t="s">
+        <v>7</v>
+      </c>
+      <c r="R3" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="S3" s="11" t="s">
+        <v>3</v>
+      </c>
+      <c r="T3" s="19" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="4" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A4" s="2">
         <v>-3.01366974606292</v>
       </c>
@@ -524,8 +905,39 @@
       <c r="I4" s="2">
         <v>-1.33419960279175</v>
       </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="K4" s="4">
+        <v>2</v>
+      </c>
+      <c r="L4" s="18">
+        <f t="shared" si="1"/>
+        <v>60</v>
+      </c>
+      <c r="M4" s="11">
+        <f t="shared" si="0"/>
+        <v>28</v>
+      </c>
+      <c r="N4" s="11">
+        <f t="shared" si="0"/>
+        <v>44</v>
+      </c>
+      <c r="O4" s="19">
+        <f t="shared" si="0"/>
+        <v>12</v>
+      </c>
+      <c r="Q4" s="18" t="s">
+        <v>10</v>
+      </c>
+      <c r="R4" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="S4" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="T4" s="19" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="5" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A5" s="2">
         <v>-1.2483028813327399</v>
       </c>
@@ -551,8 +963,39 @@
       <c r="I5" s="2">
         <v>-1.0516649878667399</v>
       </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="K5" s="4">
+        <v>3</v>
+      </c>
+      <c r="L5" s="18">
+        <f t="shared" si="1"/>
+        <v>52</v>
+      </c>
+      <c r="M5" s="11">
+        <f t="shared" si="0"/>
+        <v>20</v>
+      </c>
+      <c r="N5" s="11">
+        <f t="shared" si="0"/>
+        <v>36</v>
+      </c>
+      <c r="O5" s="19">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="Q5" s="18" t="s">
+        <v>14</v>
+      </c>
+      <c r="R5" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="S5" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="T5" s="19" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="6" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A6" s="2">
         <v>-5.57658519380443</v>
       </c>
@@ -578,8 +1021,39 @@
       <c r="I6" s="2">
         <v>-0.87082527313601799</v>
       </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="K6" s="4">
+        <v>4</v>
+      </c>
+      <c r="L6" s="18">
+        <f t="shared" si="1"/>
+        <v>62</v>
+      </c>
+      <c r="M6" s="11">
+        <f t="shared" si="0"/>
+        <v>30</v>
+      </c>
+      <c r="N6" s="11">
+        <f t="shared" si="0"/>
+        <v>46</v>
+      </c>
+      <c r="O6" s="19">
+        <f t="shared" si="0"/>
+        <v>14</v>
+      </c>
+      <c r="Q6" s="18" t="s">
+        <v>18</v>
+      </c>
+      <c r="R6" s="11" t="s">
+        <v>19</v>
+      </c>
+      <c r="S6" s="11" t="s">
+        <v>20</v>
+      </c>
+      <c r="T6" s="19" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="7" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A7" s="2">
         <v>-1.4354342058946901</v>
       </c>
@@ -605,8 +1079,39 @@
       <c r="I7" s="2">
         <v>-0.73648238794566001</v>
       </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="K7" s="4">
+        <v>5</v>
+      </c>
+      <c r="L7" s="18">
+        <f t="shared" si="1"/>
+        <v>54</v>
+      </c>
+      <c r="M7" s="11">
+        <f t="shared" si="0"/>
+        <v>22</v>
+      </c>
+      <c r="N7" s="11">
+        <f t="shared" si="0"/>
+        <v>38</v>
+      </c>
+      <c r="O7" s="19">
+        <f t="shared" si="0"/>
+        <v>6</v>
+      </c>
+      <c r="Q7" s="18" t="s">
+        <v>22</v>
+      </c>
+      <c r="R7" s="11" t="s">
+        <v>23</v>
+      </c>
+      <c r="S7" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="T7" s="19" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="8" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A8" s="2">
         <v>-2.14827910446916</v>
       </c>
@@ -632,8 +1137,39 @@
       <c r="I8" s="2">
         <v>-0.625243480095653</v>
       </c>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="K8" s="4">
+        <v>6</v>
+      </c>
+      <c r="L8" s="18">
+        <f t="shared" si="1"/>
+        <v>58</v>
+      </c>
+      <c r="M8" s="11">
+        <f t="shared" si="0"/>
+        <v>26</v>
+      </c>
+      <c r="N8" s="11">
+        <f t="shared" si="0"/>
+        <v>42</v>
+      </c>
+      <c r="O8" s="19">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+      <c r="Q8" s="18" t="s">
+        <v>26</v>
+      </c>
+      <c r="R8" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="S8" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="T8" s="19" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="9" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A9" s="2">
         <v>-1.10925176279399</v>
       </c>
@@ -659,8 +1195,39 @@
       <c r="I9" s="2">
         <v>-0.52456342488473395</v>
       </c>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="K9" s="4">
+        <v>7</v>
+      </c>
+      <c r="L9" s="18">
+        <f t="shared" si="1"/>
+        <v>50</v>
+      </c>
+      <c r="M9" s="11">
+        <f t="shared" si="0"/>
+        <v>18</v>
+      </c>
+      <c r="N9" s="11">
+        <f t="shared" si="0"/>
+        <v>34</v>
+      </c>
+      <c r="O9" s="19">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="Q9" s="18" t="s">
+        <v>30</v>
+      </c>
+      <c r="R9" s="11" t="s">
+        <v>31</v>
+      </c>
+      <c r="S9" s="11" t="s">
+        <v>32</v>
+      </c>
+      <c r="T9" s="19" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="10" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A10" s="2">
         <v>-10.677733812493599</v>
       </c>
@@ -686,8 +1253,39 @@
       <c r="I10" s="2">
         <v>-0.42583200623082601</v>
       </c>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="K10" s="4">
+        <v>8</v>
+      </c>
+      <c r="L10" s="18">
+        <f t="shared" si="1"/>
+        <v>63</v>
+      </c>
+      <c r="M10" s="11">
+        <f t="shared" si="0"/>
+        <v>31</v>
+      </c>
+      <c r="N10" s="11">
+        <f t="shared" si="0"/>
+        <v>47</v>
+      </c>
+      <c r="O10" s="19">
+        <f t="shared" si="0"/>
+        <v>15</v>
+      </c>
+      <c r="Q10" s="18" t="s">
+        <v>34</v>
+      </c>
+      <c r="R10" s="11" t="s">
+        <v>35</v>
+      </c>
+      <c r="S10" s="11" t="s">
+        <v>36</v>
+      </c>
+      <c r="T10" s="19" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="11" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A11" s="2">
         <v>-1.55716117877432</v>
       </c>
@@ -713,8 +1311,39 @@
       <c r="I11" s="2">
         <v>-0.32109713934273798</v>
       </c>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="K11" s="4">
+        <v>9</v>
+      </c>
+      <c r="L11" s="18">
+        <f t="shared" si="1"/>
+        <v>55</v>
+      </c>
+      <c r="M11" s="11">
+        <f t="shared" si="0"/>
+        <v>23</v>
+      </c>
+      <c r="N11" s="11">
+        <f t="shared" si="0"/>
+        <v>39</v>
+      </c>
+      <c r="O11" s="19">
+        <f t="shared" si="0"/>
+        <v>7</v>
+      </c>
+      <c r="Q11" s="18" t="s">
+        <v>38</v>
+      </c>
+      <c r="R11" s="11" t="s">
+        <v>39</v>
+      </c>
+      <c r="S11" s="11" t="s">
+        <v>40</v>
+      </c>
+      <c r="T11" s="19" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="12" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A12" s="2">
         <v>-2.49611189188504</v>
       </c>
@@ -740,8 +1369,39 @@
       <c r="I12" s="2">
         <v>-0.20031153315903799</v>
       </c>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="K12" s="4">
+        <v>10</v>
+      </c>
+      <c r="L12" s="18">
+        <f t="shared" si="1"/>
+        <v>59</v>
+      </c>
+      <c r="M12" s="11">
+        <f t="shared" si="0"/>
+        <v>27</v>
+      </c>
+      <c r="N12" s="11">
+        <f t="shared" si="0"/>
+        <v>43</v>
+      </c>
+      <c r="O12" s="19">
+        <f t="shared" si="0"/>
+        <v>11</v>
+      </c>
+      <c r="Q12" s="18" t="s">
+        <v>43</v>
+      </c>
+      <c r="R12" s="11" t="s">
+        <v>42</v>
+      </c>
+      <c r="S12" s="11" t="s">
+        <v>44</v>
+      </c>
+      <c r="T12" s="19" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="13" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A13" s="2">
         <v>-1.1741719567433599</v>
       </c>
@@ -767,8 +1427,39 @@
       <c r="I13" s="2">
         <v>-4.6826415490425703E-2</v>
       </c>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="K13" s="4">
+        <v>11</v>
+      </c>
+      <c r="L13" s="18">
+        <f t="shared" si="1"/>
+        <v>51</v>
+      </c>
+      <c r="M13" s="11">
+        <f t="shared" si="0"/>
+        <v>19</v>
+      </c>
+      <c r="N13" s="11">
+        <f t="shared" si="0"/>
+        <v>35</v>
+      </c>
+      <c r="O13" s="19">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="Q13" s="18" t="s">
+        <v>46</v>
+      </c>
+      <c r="R13" s="11" t="s">
+        <v>47</v>
+      </c>
+      <c r="S13" s="11" t="s">
+        <v>48</v>
+      </c>
+      <c r="T13" s="19" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="14" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A14" s="2">
         <v>-3.8707262027075</v>
       </c>
@@ -794,8 +1485,33 @@
       <c r="I14" s="2">
         <v>0.17417195674336</v>
       </c>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="K14" s="4">
+        <v>12</v>
+      </c>
+      <c r="L14" s="18">
+        <f t="shared" si="1"/>
+        <v>61</v>
+      </c>
+      <c r="M14" s="11">
+        <f t="shared" si="0"/>
+        <v>29</v>
+      </c>
+      <c r="N14" s="11">
+        <f t="shared" si="0"/>
+        <v>45</v>
+      </c>
+      <c r="O14" s="19">
+        <f t="shared" si="0"/>
+        <v>13</v>
+      </c>
+      <c r="Q14" s="18" t="s">
+        <v>50</v>
+      </c>
+      <c r="R14" s="11"/>
+      <c r="S14" s="11"/>
+      <c r="T14" s="19"/>
+    </row>
+    <row r="15" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A15" s="2">
         <v>-1.33419960279175</v>
       </c>
@@ -821,8 +1537,33 @@
       <c r="I15" s="2">
         <v>0.55716117877432003</v>
       </c>
-    </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="K15" s="4">
+        <v>13</v>
+      </c>
+      <c r="L15" s="18">
+        <f t="shared" si="1"/>
+        <v>53</v>
+      </c>
+      <c r="M15" s="11">
+        <f t="shared" si="0"/>
+        <v>21</v>
+      </c>
+      <c r="N15" s="11">
+        <f t="shared" si="0"/>
+        <v>37</v>
+      </c>
+      <c r="O15" s="19">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+      <c r="Q15" s="18" t="s">
+        <v>51</v>
+      </c>
+      <c r="R15" s="11"/>
+      <c r="S15" s="11"/>
+      <c r="T15" s="19"/>
+    </row>
+    <row r="16" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A16" s="2">
         <v>-1.8974063862452399</v>
       </c>
@@ -848,6 +1589,31 @@
       <c r="I16" s="2">
         <v>1.49611189188504</v>
       </c>
+      <c r="K16" s="4">
+        <v>14</v>
+      </c>
+      <c r="L16" s="18">
+        <f t="shared" si="1"/>
+        <v>57</v>
+      </c>
+      <c r="M16" s="11">
+        <f t="shared" si="0"/>
+        <v>25</v>
+      </c>
+      <c r="N16" s="11">
+        <f t="shared" si="0"/>
+        <v>41</v>
+      </c>
+      <c r="O16" s="19">
+        <f t="shared" si="0"/>
+        <v>9</v>
+      </c>
+      <c r="Q16" s="18" t="s">
+        <v>52</v>
+      </c>
+      <c r="R16" s="11"/>
+      <c r="S16" s="11"/>
+      <c r="T16" s="19"/>
     </row>
     <row r="17" spans="1:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="2">
@@ -875,10 +1641,47 @@
       <c r="I17" s="2">
         <v>9.6777338124935905</v>
       </c>
+      <c r="K17" s="5">
+        <v>15</v>
+      </c>
+      <c r="L17" s="20">
+        <f t="shared" si="1"/>
+        <v>49</v>
+      </c>
+      <c r="M17" s="21">
+        <f t="shared" si="0"/>
+        <v>17</v>
+      </c>
+      <c r="N17" s="21">
+        <f t="shared" si="0"/>
+        <v>33</v>
+      </c>
+      <c r="O17" s="22">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="Q17" s="20" t="s">
+        <v>53</v>
+      </c>
+      <c r="R17" s="21"/>
+      <c r="S17" s="21"/>
+      <c r="T17" s="22"/>
     </row>
     <row r="18" spans="1:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="13">
+        <v>0</v>
+      </c>
+      <c r="B18" s="14">
+        <v>1</v>
+      </c>
+      <c r="C18" s="14">
+        <v>2</v>
+      </c>
+      <c r="D18" s="14">
+        <v>3</v>
+      </c>
       <c r="E18" s="6" t="s">
-        <v>2</v>
+        <v>54</v>
       </c>
     </row>
     <row r="19" spans="1:24" x14ac:dyDescent="0.25">
@@ -918,15 +1721,15 @@
         <v>000000</v>
       </c>
       <c r="L19" t="str">
-        <f t="shared" ref="L19:N34" si="0">DEC2BIN(B19,6)</f>
+        <f t="shared" ref="L19:N34" si="2">DEC2BIN(B19,6)</f>
         <v>100000</v>
       </c>
       <c r="M19" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>010000</v>
       </c>
       <c r="N19" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>110000</v>
       </c>
       <c r="O19" s="10">
@@ -958,15 +1761,15 @@
         <v>0</v>
       </c>
       <c r="V19">
-        <f t="shared" ref="V19:X34" si="1">BIN2DEC(Q19)</f>
+        <f t="shared" ref="V19:X34" si="3">BIN2DEC(Q19)</f>
         <v>1</v>
       </c>
       <c r="W19">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>2</v>
       </c>
       <c r="X19">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>3</v>
       </c>
     </row>
@@ -999,23 +1802,23 @@
         <v>7</v>
       </c>
       <c r="J20" s="4" t="str">
-        <f t="shared" ref="J20:J34" si="2">DEC2BIN(E20,4)</f>
+        <f t="shared" ref="J20:J34" si="4">DEC2BIN(E20,4)</f>
         <v>0001</v>
       </c>
       <c r="K20" t="str">
-        <f t="shared" ref="K20:K34" si="3">DEC2BIN(A20,6)</f>
+        <f t="shared" ref="K20:K34" si="5">DEC2BIN(A20,6)</f>
         <v>001000</v>
       </c>
       <c r="L20" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>101000</v>
       </c>
       <c r="M20" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>011000</v>
       </c>
       <c r="N20" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>111000</v>
       </c>
       <c r="O20" s="8">
@@ -1039,23 +1842,23 @@
         <v>111</v>
       </c>
       <c r="T20" s="8">
-        <f t="shared" ref="T20:T34" si="4">BIN2DEC(O20)</f>
+        <f t="shared" ref="T20:T34" si="6">BIN2DEC(O20)</f>
         <v>8</v>
       </c>
       <c r="U20">
-        <f t="shared" ref="U20:U34" si="5">BIN2DEC(P20)</f>
+        <f t="shared" ref="U20:U34" si="7">BIN2DEC(P20)</f>
         <v>4</v>
       </c>
       <c r="V20">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>5</v>
       </c>
       <c r="W20">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>6</v>
       </c>
       <c r="X20">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>7</v>
       </c>
     </row>
@@ -1088,23 +1891,23 @@
         <v>11</v>
       </c>
       <c r="J21" s="4" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>0010</v>
       </c>
       <c r="K21" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>000100</v>
       </c>
       <c r="L21" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>100100</v>
       </c>
       <c r="M21" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>010100</v>
       </c>
       <c r="N21" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>110100</v>
       </c>
       <c r="O21" s="8">
@@ -1128,23 +1931,23 @@
         <v>1011</v>
       </c>
       <c r="T21" s="8">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>4</v>
       </c>
       <c r="U21">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>8</v>
       </c>
       <c r="V21">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>9</v>
       </c>
       <c r="W21">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>10</v>
       </c>
       <c r="X21">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>11</v>
       </c>
     </row>
@@ -1177,23 +1980,23 @@
         <v>15</v>
       </c>
       <c r="J22" s="4" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>0011</v>
       </c>
       <c r="K22" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>001100</v>
       </c>
       <c r="L22" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>101100</v>
       </c>
       <c r="M22" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>011100</v>
       </c>
       <c r="N22" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>111100</v>
       </c>
       <c r="O22" s="8">
@@ -1217,23 +2020,23 @@
         <v>1111</v>
       </c>
       <c r="T22" s="8">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>12</v>
       </c>
       <c r="U22">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>12</v>
       </c>
       <c r="V22">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>13</v>
       </c>
       <c r="W22">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>14</v>
       </c>
       <c r="X22">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>15</v>
       </c>
     </row>
@@ -1266,23 +2069,23 @@
         <v>19</v>
       </c>
       <c r="J23" s="4" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>0100</v>
       </c>
       <c r="K23" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>000010</v>
       </c>
       <c r="L23" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>100010</v>
       </c>
       <c r="M23" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>010010</v>
       </c>
       <c r="N23" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>110010</v>
       </c>
       <c r="O23" s="8">
@@ -1306,23 +2109,23 @@
         <v>10011</v>
       </c>
       <c r="T23" s="8">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>2</v>
       </c>
       <c r="U23">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>16</v>
       </c>
       <c r="V23">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>17</v>
       </c>
       <c r="W23">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>18</v>
       </c>
       <c r="X23">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>19</v>
       </c>
     </row>
@@ -1355,23 +2158,23 @@
         <v>23</v>
       </c>
       <c r="J24" s="4" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>0101</v>
       </c>
       <c r="K24" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>001010</v>
       </c>
       <c r="L24" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>101010</v>
       </c>
       <c r="M24" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>011010</v>
       </c>
       <c r="N24" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>111010</v>
       </c>
       <c r="O24" s="8">
@@ -1395,23 +2198,23 @@
         <v>10111</v>
       </c>
       <c r="T24" s="8">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>10</v>
       </c>
       <c r="U24">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>20</v>
       </c>
       <c r="V24">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>21</v>
       </c>
       <c r="W24">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>22</v>
       </c>
       <c r="X24">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>23</v>
       </c>
     </row>
@@ -1444,23 +2247,23 @@
         <v>27</v>
       </c>
       <c r="J25" s="4" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>0110</v>
       </c>
       <c r="K25" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>000110</v>
       </c>
       <c r="L25" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>100110</v>
       </c>
       <c r="M25" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>010110</v>
       </c>
       <c r="N25" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>110110</v>
       </c>
       <c r="O25" s="8">
@@ -1484,23 +2287,23 @@
         <v>11011</v>
       </c>
       <c r="T25" s="8">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>6</v>
       </c>
       <c r="U25">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>24</v>
       </c>
       <c r="V25">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>25</v>
       </c>
       <c r="W25">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>26</v>
       </c>
       <c r="X25">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>27</v>
       </c>
     </row>
@@ -1533,23 +2336,23 @@
         <v>31</v>
       </c>
       <c r="J26" s="4" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>0111</v>
       </c>
       <c r="K26" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>001110</v>
       </c>
       <c r="L26" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>101110</v>
       </c>
       <c r="M26" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>011110</v>
       </c>
       <c r="N26" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>111110</v>
       </c>
       <c r="O26" s="8">
@@ -1573,23 +2376,23 @@
         <v>11111</v>
       </c>
       <c r="T26" s="8">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>14</v>
       </c>
       <c r="U26">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>28</v>
       </c>
       <c r="V26">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>29</v>
       </c>
       <c r="W26">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>30</v>
       </c>
       <c r="X26">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>31</v>
       </c>
     </row>
@@ -1622,23 +2425,23 @@
         <v>35</v>
       </c>
       <c r="J27" s="4" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>1000</v>
       </c>
       <c r="K27" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>000001</v>
       </c>
       <c r="L27" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>100001</v>
       </c>
       <c r="M27" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>010001</v>
       </c>
       <c r="N27" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>110001</v>
       </c>
       <c r="O27" s="8">
@@ -1662,23 +2465,23 @@
         <v>100011</v>
       </c>
       <c r="T27" s="8">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>1</v>
       </c>
       <c r="U27">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>32</v>
       </c>
       <c r="V27">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>33</v>
       </c>
       <c r="W27">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>34</v>
       </c>
       <c r="X27">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>35</v>
       </c>
     </row>
@@ -1711,23 +2514,23 @@
         <v>39</v>
       </c>
       <c r="J28" s="4" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>1001</v>
       </c>
       <c r="K28" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>001001</v>
       </c>
       <c r="L28" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>101001</v>
       </c>
       <c r="M28" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>011001</v>
       </c>
       <c r="N28" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>111001</v>
       </c>
       <c r="O28" s="8">
@@ -1751,23 +2554,23 @@
         <v>100111</v>
       </c>
       <c r="T28" s="8">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>9</v>
       </c>
       <c r="U28">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>36</v>
       </c>
       <c r="V28">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>37</v>
       </c>
       <c r="W28">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>38</v>
       </c>
       <c r="X28">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>39</v>
       </c>
     </row>
@@ -1800,23 +2603,23 @@
         <v>43</v>
       </c>
       <c r="J29" s="4" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>1010</v>
       </c>
       <c r="K29" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>000101</v>
       </c>
       <c r="L29" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>100101</v>
       </c>
       <c r="M29" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>010101</v>
       </c>
       <c r="N29" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>110101</v>
       </c>
       <c r="O29" s="8">
@@ -1840,23 +2643,23 @@
         <v>101011</v>
       </c>
       <c r="T29" s="8">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>5</v>
       </c>
       <c r="U29">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>40</v>
       </c>
       <c r="V29">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>41</v>
       </c>
       <c r="W29">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>42</v>
       </c>
       <c r="X29">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>43</v>
       </c>
     </row>
@@ -1889,23 +2692,23 @@
         <v>47</v>
       </c>
       <c r="J30" s="4" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>1011</v>
       </c>
       <c r="K30" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>001101</v>
       </c>
       <c r="L30" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>101101</v>
       </c>
       <c r="M30" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>011101</v>
       </c>
       <c r="N30" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>111101</v>
       </c>
       <c r="O30" s="8">
@@ -1929,23 +2732,23 @@
         <v>101111</v>
       </c>
       <c r="T30" s="8">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>13</v>
       </c>
       <c r="U30">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>44</v>
       </c>
       <c r="V30">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>45</v>
       </c>
       <c r="W30">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>46</v>
       </c>
       <c r="X30">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>47</v>
       </c>
     </row>
@@ -1978,23 +2781,23 @@
         <v>51</v>
       </c>
       <c r="J31" s="4" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>1100</v>
       </c>
       <c r="K31" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>000011</v>
       </c>
       <c r="L31" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>100011</v>
       </c>
       <c r="M31" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>010011</v>
       </c>
       <c r="N31" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>110011</v>
       </c>
       <c r="O31" s="8">
@@ -2018,23 +2821,23 @@
         <v>110011</v>
       </c>
       <c r="T31" s="8">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>3</v>
       </c>
       <c r="U31">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>48</v>
       </c>
       <c r="V31">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>49</v>
       </c>
       <c r="W31">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>50</v>
       </c>
       <c r="X31">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>51</v>
       </c>
     </row>
@@ -2067,23 +2870,23 @@
         <v>55</v>
       </c>
       <c r="J32" s="4" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>1101</v>
       </c>
       <c r="K32" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>001011</v>
       </c>
       <c r="L32" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>101011</v>
       </c>
       <c r="M32" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>011011</v>
       </c>
       <c r="N32" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>111011</v>
       </c>
       <c r="O32" s="8">
@@ -2107,23 +2910,23 @@
         <v>110111</v>
       </c>
       <c r="T32" s="8">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>11</v>
       </c>
       <c r="U32">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>52</v>
       </c>
       <c r="V32">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>53</v>
       </c>
       <c r="W32">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>54</v>
       </c>
       <c r="X32">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>55</v>
       </c>
     </row>
@@ -2156,23 +2959,23 @@
         <v>59</v>
       </c>
       <c r="J33" s="4" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>1110</v>
       </c>
       <c r="K33" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>000111</v>
       </c>
       <c r="L33" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>100111</v>
       </c>
       <c r="M33" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>010111</v>
       </c>
       <c r="N33" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>110111</v>
       </c>
       <c r="O33" s="8">
@@ -2196,23 +2999,23 @@
         <v>111011</v>
       </c>
       <c r="T33" s="8">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>7</v>
       </c>
       <c r="U33">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>56</v>
       </c>
       <c r="V33">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>57</v>
       </c>
       <c r="W33">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>58</v>
       </c>
       <c r="X33">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>59</v>
       </c>
     </row>
@@ -2245,23 +3048,23 @@
         <v>63</v>
       </c>
       <c r="J34" s="5" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>1111</v>
       </c>
       <c r="K34" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>001111</v>
       </c>
       <c r="L34" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>101111</v>
       </c>
       <c r="M34" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>011111</v>
       </c>
       <c r="N34" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>111111</v>
       </c>
       <c r="O34" s="9">
@@ -2285,23 +3088,23 @@
         <v>111111</v>
       </c>
       <c r="T34" s="9">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>15</v>
       </c>
       <c r="U34">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>60</v>
       </c>
       <c r="V34">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>61</v>
       </c>
       <c r="W34">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>62</v>
       </c>
       <c r="X34">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>63</v>
       </c>
     </row>

</xml_diff>

<commit_message>
fix save reg ver of ram from matlab
</commit_message>
<xml_diff>
--- a/docs/ram.xlsx
+++ b/docs/ram.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\work\fpga\fht\docs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\work\src_fpga\fht\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -229,12 +229,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="16">
@@ -418,7 +424,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -444,6 +450,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
@@ -724,10 +733,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:X38"/>
+  <dimension ref="A1:AC38"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="Q2" sqref="Q2"/>
+      <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -735,7 +744,7 @@
     <col min="5" max="5" width="9.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:29" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -764,7 +773,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="2" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:29" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="2">
         <v>31.5</v>
       </c>
@@ -820,8 +829,20 @@
       <c r="T2" s="17" t="s">
         <v>6</v>
       </c>
+      <c r="Z2">
+        <v>0</v>
+      </c>
+      <c r="AA2">
+        <v>1</v>
+      </c>
+      <c r="AB2">
+        <v>2</v>
+      </c>
+      <c r="AC2">
+        <v>3</v>
+      </c>
     </row>
-    <row r="3" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A3" s="2">
         <v>-1.7071067811865499</v>
       </c>
@@ -878,8 +899,23 @@
       <c r="T3" s="19" t="s">
         <v>9</v>
       </c>
+      <c r="Y3">
+        <v>0</v>
+      </c>
+      <c r="Z3" s="15">
+        <v>0</v>
+      </c>
+      <c r="AA3" s="16">
+        <v>32</v>
+      </c>
+      <c r="AB3" s="16">
+        <v>16</v>
+      </c>
+      <c r="AC3" s="17">
+        <v>48</v>
+      </c>
     </row>
-    <row r="4" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A4" s="2">
         <v>-3.01366974606292</v>
       </c>
@@ -936,8 +972,23 @@
       <c r="T4" s="19" t="s">
         <v>13</v>
       </c>
+      <c r="Y4">
+        <v>1</v>
+      </c>
+      <c r="Z4" s="18">
+        <v>1</v>
+      </c>
+      <c r="AA4" s="11">
+        <v>33</v>
+      </c>
+      <c r="AB4" s="11">
+        <v>17</v>
+      </c>
+      <c r="AC4" s="19">
+        <v>49</v>
+      </c>
     </row>
-    <row r="5" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A5" s="2">
         <v>-1.2483028813327399</v>
       </c>
@@ -994,8 +1045,23 @@
       <c r="T5" s="19" t="s">
         <v>17</v>
       </c>
+      <c r="Y5">
+        <v>2</v>
+      </c>
+      <c r="Z5" s="18">
+        <v>2</v>
+      </c>
+      <c r="AA5" s="11">
+        <v>34</v>
+      </c>
+      <c r="AB5" s="11">
+        <v>18</v>
+      </c>
+      <c r="AC5" s="19">
+        <v>50</v>
+      </c>
     </row>
-    <row r="6" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A6" s="2">
         <v>-5.57658519380443</v>
       </c>
@@ -1052,8 +1118,23 @@
       <c r="T6" s="19" t="s">
         <v>21</v>
       </c>
+      <c r="Y6">
+        <v>3</v>
+      </c>
+      <c r="Z6" s="18">
+        <v>3</v>
+      </c>
+      <c r="AA6" s="11">
+        <v>35</v>
+      </c>
+      <c r="AB6" s="11">
+        <v>19</v>
+      </c>
+      <c r="AC6" s="19">
+        <v>51</v>
+      </c>
     </row>
-    <row r="7" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A7" s="2">
         <v>-1.4354342058946901</v>
       </c>
@@ -1110,8 +1191,23 @@
       <c r="T7" s="19" t="s">
         <v>25</v>
       </c>
+      <c r="Y7">
+        <v>4</v>
+      </c>
+      <c r="Z7" s="25">
+        <v>4</v>
+      </c>
+      <c r="AA7" s="26">
+        <v>36</v>
+      </c>
+      <c r="AB7" s="11">
+        <v>20</v>
+      </c>
+      <c r="AC7" s="19">
+        <v>52</v>
+      </c>
     </row>
-    <row r="8" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A8" s="2">
         <v>-2.14827910446916</v>
       </c>
@@ -1168,8 +1264,23 @@
       <c r="T8" s="19" t="s">
         <v>29</v>
       </c>
+      <c r="Y8">
+        <v>5</v>
+      </c>
+      <c r="Z8" s="18">
+        <v>5</v>
+      </c>
+      <c r="AA8" s="11">
+        <v>37</v>
+      </c>
+      <c r="AB8" s="11">
+        <v>21</v>
+      </c>
+      <c r="AC8" s="19">
+        <v>53</v>
+      </c>
     </row>
-    <row r="9" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A9" s="2">
         <v>-1.10925176279399</v>
       </c>
@@ -1226,8 +1337,23 @@
       <c r="T9" s="19" t="s">
         <v>33</v>
       </c>
+      <c r="Y9">
+        <v>6</v>
+      </c>
+      <c r="Z9" s="18">
+        <v>6</v>
+      </c>
+      <c r="AA9" s="11">
+        <v>38</v>
+      </c>
+      <c r="AB9" s="11">
+        <v>22</v>
+      </c>
+      <c r="AC9" s="19">
+        <v>54</v>
+      </c>
     </row>
-    <row r="10" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A10" s="2">
         <v>-10.677733812493599</v>
       </c>
@@ -1284,8 +1410,23 @@
       <c r="T10" s="19" t="s">
         <v>37</v>
       </c>
+      <c r="Y10">
+        <v>7</v>
+      </c>
+      <c r="Z10" s="18">
+        <v>7</v>
+      </c>
+      <c r="AA10" s="11">
+        <v>39</v>
+      </c>
+      <c r="AB10" s="11">
+        <v>23</v>
+      </c>
+      <c r="AC10" s="19">
+        <v>55</v>
+      </c>
     </row>
-    <row r="11" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A11" s="2">
         <v>-1.55716117877432</v>
       </c>
@@ -1342,8 +1483,23 @@
       <c r="T11" s="19" t="s">
         <v>41</v>
       </c>
+      <c r="Y11">
+        <v>8</v>
+      </c>
+      <c r="Z11" s="25">
+        <v>8</v>
+      </c>
+      <c r="AA11" s="26">
+        <v>40</v>
+      </c>
+      <c r="AB11" s="26">
+        <v>24</v>
+      </c>
+      <c r="AC11" s="27">
+        <v>56</v>
+      </c>
     </row>
-    <row r="12" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A12" s="2">
         <v>-2.49611189188504</v>
       </c>
@@ -1400,8 +1556,23 @@
       <c r="T12" s="19" t="s">
         <v>45</v>
       </c>
+      <c r="Y12">
+        <v>9</v>
+      </c>
+      <c r="Z12" s="18">
+        <v>9</v>
+      </c>
+      <c r="AA12" s="11">
+        <v>41</v>
+      </c>
+      <c r="AB12" s="11">
+        <v>25</v>
+      </c>
+      <c r="AC12" s="19">
+        <v>57</v>
+      </c>
     </row>
-    <row r="13" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A13" s="2">
         <v>-1.1741719567433599</v>
       </c>
@@ -1458,8 +1629,23 @@
       <c r="T13" s="19" t="s">
         <v>49</v>
       </c>
+      <c r="Y13">
+        <v>10</v>
+      </c>
+      <c r="Z13" s="18">
+        <v>10</v>
+      </c>
+      <c r="AA13" s="11">
+        <v>42</v>
+      </c>
+      <c r="AB13" s="11">
+        <v>26</v>
+      </c>
+      <c r="AC13" s="19">
+        <v>58</v>
+      </c>
     </row>
-    <row r="14" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A14" s="2">
         <v>-3.8707262027075</v>
       </c>
@@ -1510,8 +1696,23 @@
       <c r="R14" s="11"/>
       <c r="S14" s="11"/>
       <c r="T14" s="19"/>
+      <c r="Y14">
+        <v>11</v>
+      </c>
+      <c r="Z14" s="18">
+        <v>11</v>
+      </c>
+      <c r="AA14" s="11">
+        <v>43</v>
+      </c>
+      <c r="AB14" s="11">
+        <v>27</v>
+      </c>
+      <c r="AC14" s="19">
+        <v>59</v>
+      </c>
     </row>
-    <row r="15" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A15" s="2">
         <v>-1.33419960279175</v>
       </c>
@@ -1562,8 +1763,23 @@
       <c r="R15" s="11"/>
       <c r="S15" s="11"/>
       <c r="T15" s="19"/>
+      <c r="Y15">
+        <v>12</v>
+      </c>
+      <c r="Z15" s="18">
+        <v>12</v>
+      </c>
+      <c r="AA15" s="11">
+        <v>44</v>
+      </c>
+      <c r="AB15" s="11">
+        <v>28</v>
+      </c>
+      <c r="AC15" s="19">
+        <v>60</v>
+      </c>
     </row>
-    <row r="16" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A16" s="2">
         <v>-1.8974063862452399</v>
       </c>
@@ -1614,8 +1830,23 @@
       <c r="R16" s="11"/>
       <c r="S16" s="11"/>
       <c r="T16" s="19"/>
+      <c r="Y16">
+        <v>13</v>
+      </c>
+      <c r="Z16" s="18">
+        <v>13</v>
+      </c>
+      <c r="AA16" s="11">
+        <v>45</v>
+      </c>
+      <c r="AB16" s="11">
+        <v>29</v>
+      </c>
+      <c r="AC16" s="19">
+        <v>61</v>
+      </c>
     </row>
-    <row r="17" spans="1:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:29" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="2">
         <v>-1.0516649878667399</v>
       </c>
@@ -1666,8 +1897,23 @@
       <c r="R17" s="21"/>
       <c r="S17" s="21"/>
       <c r="T17" s="22"/>
+      <c r="Y17">
+        <v>14</v>
+      </c>
+      <c r="Z17" s="18">
+        <v>14</v>
+      </c>
+      <c r="AA17" s="11">
+        <v>46</v>
+      </c>
+      <c r="AB17" s="11">
+        <v>30</v>
+      </c>
+      <c r="AC17" s="19">
+        <v>62</v>
+      </c>
     </row>
-    <row r="18" spans="1:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:29" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="13">
         <v>0</v>
       </c>
@@ -1683,8 +1929,23 @@
       <c r="E18" s="6" t="s">
         <v>54</v>
       </c>
+      <c r="Y18">
+        <v>15</v>
+      </c>
+      <c r="Z18" s="20">
+        <v>15</v>
+      </c>
+      <c r="AA18" s="21">
+        <v>47</v>
+      </c>
+      <c r="AB18" s="21">
+        <v>31</v>
+      </c>
+      <c r="AC18" s="22">
+        <v>63</v>
+      </c>
     </row>
-    <row r="19" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A19" s="2">
         <v>0</v>
       </c>
@@ -1773,7 +2034,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="20" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A20" s="2">
         <v>8</v>
       </c>
@@ -1861,8 +2122,23 @@
         <f t="shared" si="3"/>
         <v>7</v>
       </c>
+      <c r="Z20">
+        <v>0</v>
+      </c>
+      <c r="AA20" t="str">
+        <f>DEC2BIN(Z20,6)</f>
+        <v>000000</v>
+      </c>
+      <c r="AB20">
+        <f>SUMPRODUCT(MID($AA20,{1;2;3;4;5;6},1)*10^{0;1;2;3;4;5})</f>
+        <v>0</v>
+      </c>
+      <c r="AC20">
+        <f>BIN2DEC(AB20)</f>
+        <v>0</v>
+      </c>
     </row>
-    <row r="21" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A21" s="2">
         <v>4</v>
       </c>
@@ -1950,8 +2226,23 @@
         <f t="shared" si="3"/>
         <v>11</v>
       </c>
+      <c r="Z21">
+        <v>8</v>
+      </c>
+      <c r="AA21" t="str">
+        <f t="shared" ref="AA21:AA29" si="8">DEC2BIN(Z21,6)</f>
+        <v>001000</v>
+      </c>
+      <c r="AB21">
+        <f>SUMPRODUCT(MID($AA21,{1;2;3;4;5;6},1)*10^{0;1;2;3;4;5})</f>
+        <v>100</v>
+      </c>
+      <c r="AC21">
+        <f t="shared" ref="AC21:AC29" si="9">BIN2DEC(AB21)</f>
+        <v>4</v>
+      </c>
     </row>
-    <row r="22" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A22" s="2">
         <v>12</v>
       </c>
@@ -2039,8 +2330,23 @@
         <f t="shared" si="3"/>
         <v>15</v>
       </c>
+      <c r="Z22">
+        <v>12</v>
+      </c>
+      <c r="AA22" t="str">
+        <f t="shared" si="8"/>
+        <v>001100</v>
+      </c>
+      <c r="AB22">
+        <f>SUMPRODUCT(MID($AA22,{1;2;3;4;5;6},1)*10^{0;1;2;3;4;5})</f>
+        <v>1100</v>
+      </c>
+      <c r="AC22">
+        <f t="shared" si="9"/>
+        <v>12</v>
+      </c>
     </row>
-    <row r="23" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A23" s="2">
         <v>2</v>
       </c>
@@ -2128,8 +2434,23 @@
         <f t="shared" si="3"/>
         <v>19</v>
       </c>
+      <c r="Z23">
+        <v>4</v>
+      </c>
+      <c r="AA23" t="str">
+        <f t="shared" si="8"/>
+        <v>000100</v>
+      </c>
+      <c r="AB23">
+        <f>SUMPRODUCT(MID($AA23,{1;2;3;4;5;6},1)*10^{0;1;2;3;4;5})</f>
+        <v>1000</v>
+      </c>
+      <c r="AC23">
+        <f t="shared" si="9"/>
+        <v>8</v>
+      </c>
     </row>
-    <row r="24" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A24" s="2">
         <v>10</v>
       </c>
@@ -2217,8 +2538,23 @@
         <f t="shared" si="3"/>
         <v>23</v>
       </c>
+      <c r="Z24">
+        <v>14</v>
+      </c>
+      <c r="AA24" t="str">
+        <f t="shared" si="8"/>
+        <v>001110</v>
+      </c>
+      <c r="AB24">
+        <f>SUMPRODUCT(MID($AA24,{1;2;3;4;5;6},1)*10^{0;1;2;3;4;5})</f>
+        <v>11100</v>
+      </c>
+      <c r="AC24">
+        <f t="shared" si="9"/>
+        <v>28</v>
+      </c>
     </row>
-    <row r="25" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A25" s="2">
         <v>6</v>
       </c>
@@ -2306,8 +2642,23 @@
         <f t="shared" si="3"/>
         <v>27</v>
       </c>
+      <c r="Z25">
+        <v>6</v>
+      </c>
+      <c r="AA25" t="str">
+        <f t="shared" si="8"/>
+        <v>000110</v>
+      </c>
+      <c r="AB25">
+        <f>SUMPRODUCT(MID($AA25,{1;2;3;4;5;6},1)*10^{0;1;2;3;4;5})</f>
+        <v>11000</v>
+      </c>
+      <c r="AC25">
+        <f t="shared" si="9"/>
+        <v>24</v>
+      </c>
     </row>
-    <row r="26" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A26" s="2">
         <v>14</v>
       </c>
@@ -2395,8 +2746,23 @@
         <f t="shared" si="3"/>
         <v>31</v>
       </c>
+      <c r="Z26">
+        <v>10</v>
+      </c>
+      <c r="AA26" t="str">
+        <f t="shared" si="8"/>
+        <v>001010</v>
+      </c>
+      <c r="AB26">
+        <f>SUMPRODUCT(MID($AA26,{1;2;3;4;5;6},1)*10^{0;1;2;3;4;5})</f>
+        <v>10100</v>
+      </c>
+      <c r="AC26">
+        <f t="shared" si="9"/>
+        <v>20</v>
+      </c>
     </row>
-    <row r="27" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A27" s="2">
         <v>1</v>
       </c>
@@ -2484,8 +2850,23 @@
         <f t="shared" si="3"/>
         <v>35</v>
       </c>
+      <c r="Z27">
+        <v>2</v>
+      </c>
+      <c r="AA27" t="str">
+        <f t="shared" si="8"/>
+        <v>000010</v>
+      </c>
+      <c r="AB27">
+        <f>SUMPRODUCT(MID($AA27,{1;2;3;4;5;6},1)*10^{0;1;2;3;4;5})</f>
+        <v>10000</v>
+      </c>
+      <c r="AC27">
+        <f t="shared" si="9"/>
+        <v>16</v>
+      </c>
     </row>
-    <row r="28" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A28" s="2">
         <v>9</v>
       </c>
@@ -2573,8 +2954,23 @@
         <f t="shared" si="3"/>
         <v>39</v>
       </c>
+      <c r="Z28">
+        <v>15</v>
+      </c>
+      <c r="AA28" t="str">
+        <f t="shared" si="8"/>
+        <v>001111</v>
+      </c>
+      <c r="AB28">
+        <f>SUMPRODUCT(MID($AA28,{1;2;3;4;5;6},1)*10^{0;1;2;3;4;5})</f>
+        <v>111100</v>
+      </c>
+      <c r="AC28">
+        <f t="shared" si="9"/>
+        <v>60</v>
+      </c>
     </row>
-    <row r="29" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A29" s="2">
         <v>5</v>
       </c>
@@ -2662,8 +3058,23 @@
         <f t="shared" si="3"/>
         <v>43</v>
       </c>
+      <c r="Z29">
+        <v>7</v>
+      </c>
+      <c r="AA29" t="str">
+        <f t="shared" si="8"/>
+        <v>000111</v>
+      </c>
+      <c r="AB29">
+        <f>SUMPRODUCT(MID($AA29,{1;2;3;4;5;6},1)*10^{0;1;2;3;4;5})</f>
+        <v>111000</v>
+      </c>
+      <c r="AC29">
+        <f t="shared" si="9"/>
+        <v>56</v>
+      </c>
     </row>
-    <row r="30" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A30" s="2">
         <v>13</v>
       </c>
@@ -2752,7 +3163,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="31" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A31" s="2">
         <v>3</v>
       </c>
@@ -2841,7 +3252,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="32" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A32" s="2">
         <v>11</v>
       </c>
@@ -3111,6 +3522,6 @@
     <row r="38" spans="1:24" ht="17.25" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>